<commit_message>
redmine #9137 cal sheets for CP02PMUI multiple deployments changed/added.
</commit_message>
<xml_diff>
--- a/CP02PMUI/Omaha_Cal_Info_CP02PMUI_00001.xlsx
+++ b/CP02PMUI/Omaha_Cal_Info_CP02PMUI_00001.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14055" windowHeight="5580" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="6800" yWindow="6280" windowWidth="25560" windowHeight="12540" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
     <sheet name="Asset_Cal_Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Asset_Cal_Info!$A$1:$F$33</definedName>
-    <definedName name="_xlnm._FilterDatabase">Asset_Cal_Info!$A$1:$F$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Asset_Cal_Info!$A$1:$F$35</definedName>
+    <definedName name="_xlnm._FilterDatabase">Asset_Cal_Info!$A$1:$F$35</definedName>
     <definedName name="_FilterDatabase_0">Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0">Moorings!$A$1:$J$80</definedName>
     <definedName name="_FilterDatabase_0_0_0">Moorings!#REF!</definedName>
@@ -25,17 +25,22 @@
     <definedName name="_FilterDatabase_0_0_0_1">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_0_0_1">Asset_Cal_Info!$A$1:$F$403</definedName>
     <definedName name="_FilterDatabase_0_1">Asset_Cal_Info!$A$1:$F$1</definedName>
-    <definedName name="_FilterDatabase_1">Asset_Cal_Info!$A$1:$F$33</definedName>
+    <definedName name="_FilterDatabase_1">Asset_Cal_Info!$A$1:$F$35</definedName>
     <definedName name="_FilterDatabase_1_1">Asset_Cal_Info!$A$1:$F$1</definedName>
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$80</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$403</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="71">
   <si>
     <t>Ref Des</t>
   </si>
@@ -243,9 +248,6 @@
     <t>This serial number is a placekeeper used until the correct serial number is found or defined</t>
   </si>
   <si>
-    <t>CP02PMUI-SBS01-00-RTE000000</t>
-  </si>
-  <si>
     <t>CP02PMUI-WFP01-00-WFPENG000</t>
   </si>
   <si>
@@ -294,6 +296,9 @@
       <t>-VEL3DK000</t>
     </r>
   </si>
+  <si>
+    <t>units = mm</t>
+  </si>
 </sst>
 </file>
 
@@ -302,7 +307,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -408,6 +413,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -486,11 +512,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -563,9 +597,18 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="10">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -938,28 +981,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="37.85546875"/>
-    <col min="2" max="2" width="39.42578125"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.42578125"/>
-    <col min="7" max="7" width="18.7109375"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875"/>
-    <col min="10" max="10" width="12.7109375"/>
-    <col min="11" max="11" width="51.7109375"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="1026" width="8.7109375"/>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="8" width="18.5" customWidth="1"/>
+    <col min="9" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5">
+    <row r="1" spans="1:13" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -994,7 +1034,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" ht="15">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
@@ -1026,14 +1066,8 @@
         <v>43</v>
       </c>
       <c r="K2" s="6"/>
-      <c r="L2" s="15">
-        <f>((LEFT(G2,(FIND("°",G2,1)-1)))+(MID(G2,(FIND("°",G2,1)+1),(FIND("'",G2,1))-(FIND("°",G2,1)+1))/60))*(IF(RIGHT(G2,1)="N",1,-1))</f>
-        <v>40.363405</v>
-      </c>
-      <c r="M2" s="15">
-        <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="E",1,-1))</f>
-        <v>-70.775988333333331</v>
-      </c>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13">
       <c r="D3" s="9"/>
@@ -1045,35 +1079,35 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125"/>
-    <col min="9" max="9" width="11.85546875"/>
-    <col min="10" max="10" width="14.42578125"/>
-    <col min="11" max="11" width="13.42578125"/>
-    <col min="12" max="1026" width="8.7109375"/>
+    <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1110,9 +1144,11 @@
         <v>16</v>
       </c>
       <c r="F2" s="20">
-        <v>71.97</v>
-      </c>
-      <c r="G2" s="18"/>
+        <v>73000</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>70</v>
+      </c>
       <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8">
@@ -1171,7 +1207,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="18" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>42</v>
@@ -1179,41 +1215,20 @@
       <c r="C6" s="19">
         <v>1</v>
       </c>
-      <c r="D6" s="21">
-        <v>2497</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="22">
-        <v>-837.37</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>44</v>
+      <c r="D6" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="26" t="s">
+        <v>60</v>
       </c>
       <c r="H6" s="18"/>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="19">
-        <v>1</v>
-      </c>
-      <c r="D7" s="23">
-        <v>2497</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="20">
-        <v>40.363405</v>
-      </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
+    <row r="7" spans="1:8" ht="15">
+      <c r="A7" s="8"/>
+      <c r="D7" s="16"/>
+      <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="18" t="s">
@@ -1225,16 +1240,18 @@
       <c r="C8" s="19">
         <v>1</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="21">
         <v>2497</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="20">
-        <v>-70.775988333333331</v>
-      </c>
-      <c r="G8" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="F8" s="22">
+        <v>-837.37</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8">
@@ -1251,14 +1268,12 @@
         <v>2497</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="22">
-        <v>2.5849999999999999E-4</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>45</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F9" s="20">
+        <v>40.363405</v>
+      </c>
+      <c r="G9" s="18"/>
       <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8">
@@ -1275,14 +1290,12 @@
         <v>2497</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="22">
-        <v>-3.3024999999999999E-3</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>46</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F10" s="20">
+        <v>-70.775988333333331</v>
+      </c>
+      <c r="G10" s="18"/>
       <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8">
@@ -1299,13 +1312,13 @@
         <v>2497</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11" s="22">
-        <v>1.9880000000000001E-4</v>
+        <v>2.5849999999999999E-4</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -1323,13 +1336,13 @@
         <v>2497</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F12" s="22">
-        <v>-3.0292999999999999E-6</v>
+        <v>-3.3024999999999999E-3</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -1347,29 +1360,43 @@
         <v>2497</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F13" s="22">
-        <v>3.5999999999999997E-2</v>
+        <v>1.9880000000000001E-4</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="18"/>
+      <c r="A14" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="19">
+        <v>1</v>
+      </c>
+      <c r="D14" s="23">
+        <v>2497</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="22">
+        <v>-3.0292999999999999E-6</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>48</v>
+      </c>
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="18" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>42</v>
@@ -1377,53 +1404,55 @@
       <c r="C15" s="19">
         <v>1</v>
       </c>
-      <c r="D15" s="19">
-        <v>111</v>
+      <c r="D15" s="23">
+        <v>2497</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="20">
-        <v>40.363405</v>
-      </c>
-      <c r="G15" s="18"/>
+        <v>25</v>
+      </c>
+      <c r="F15" s="22">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="19">
-        <v>1</v>
-      </c>
-      <c r="D16" s="19">
-        <v>111</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="20">
-        <v>-70.775988333333331</v>
-      </c>
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="22"/>
       <c r="G16" s="18"/>
       <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="20"/>
+      <c r="A17" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="19">
+        <v>1</v>
+      </c>
+      <c r="D17" s="19">
+        <v>111</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="20">
+        <v>40.363405</v>
+      </c>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="18" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>42</v>
@@ -1431,53 +1460,53 @@
       <c r="C18" s="19">
         <v>1</v>
       </c>
-      <c r="D18" s="23">
-        <v>100015</v>
+      <c r="D18" s="19">
+        <v>111</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F18" s="20">
-        <v>40.363405</v>
+        <v>-70.775988333333331</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="19">
-        <v>1</v>
-      </c>
-      <c r="D19" s="23">
-        <v>100015</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="20">
-        <v>-70.775988333333331</v>
-      </c>
+      <c r="A19" s="18"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="18"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="20"/>
+      <c r="A20" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="19">
+        <v>1</v>
+      </c>
+      <c r="D20" s="23">
+        <v>100015</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="20">
+        <v>40.363405</v>
+      </c>
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="18" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>42</v>
@@ -1485,42 +1514,26 @@
       <c r="C21" s="19">
         <v>1</v>
       </c>
-      <c r="D21" s="19">
-        <v>1029</v>
+      <c r="D21" s="23">
+        <v>100015</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="F21" s="20">
-        <v>1.0760000000000001</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>41</v>
-      </c>
+        <v>-70.775988333333331</v>
+      </c>
+      <c r="G21" s="18"/>
       <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="19">
-        <v>1</v>
-      </c>
-      <c r="D22" s="19">
-        <v>1029</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="20">
-        <v>50</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>50</v>
-      </c>
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:8">
@@ -1537,13 +1550,13 @@
         <v>1029</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="F23" s="20">
-        <v>53</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>51</v>
+        <v>1.0760000000000001</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="H23" s="18"/>
     </row>
@@ -1561,13 +1574,13 @@
         <v>1029</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F24" s="20">
         <v>50</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H24" s="18"/>
     </row>
@@ -1585,13 +1598,13 @@
         <v>1029</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="F25" s="20">
-        <v>3.9E-2</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>41</v>
+        <v>53</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>51</v>
       </c>
       <c r="H25" s="18"/>
     </row>
@@ -1609,13 +1622,13 @@
         <v>1029</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="F26" s="20">
-        <v>700</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>41</v>
+        <v>50</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="H26" s="18"/>
     </row>
@@ -1633,13 +1646,13 @@
         <v>1029</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="F27" s="20">
-        <v>9.0700000000000003E-2</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>53</v>
+        <v>3.9E-2</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="H27" s="18"/>
     </row>
@@ -1657,13 +1670,13 @@
         <v>1029</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="F28" s="20">
-        <v>1.21E-2</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>54</v>
+        <v>700</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>41</v>
       </c>
       <c r="H28" s="18"/>
     </row>
@@ -1681,13 +1694,13 @@
         <v>1029</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="24">
-        <v>3.49E-6</v>
+        <v>33</v>
+      </c>
+      <c r="F29" s="20">
+        <v>9.0700000000000003E-2</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H29" s="18"/>
     </row>
@@ -1705,87 +1718,101 @@
         <v>1029</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="F30" s="20">
-        <v>124</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>41</v>
+        <v>1.21E-2</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>54</v>
       </c>
       <c r="H30" s="18"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="18"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="18"/>
+      <c r="A31" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="19">
+        <v>1</v>
+      </c>
+      <c r="D31" s="19">
+        <v>1029</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="24">
+        <v>3.49E-6</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>52</v>
+      </c>
       <c r="H31" s="18"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="19">
+        <v>1</v>
+      </c>
+      <c r="D32" s="19">
+        <v>1029</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="20">
+        <v>124</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H32" s="18"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="18"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C32" s="19">
-        <v>1</v>
-      </c>
-      <c r="D32" s="19">
+      <c r="B34" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="19">
+        <v>1</v>
+      </c>
+      <c r="D34" s="19">
         <v>20437</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E34" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="20">
+      <c r="F34" s="20">
         <v>1.5</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G34" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H32" s="18"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="19">
-        <v>1</v>
-      </c>
-      <c r="D33" s="19">
-        <v>20437</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" s="24">
-        <v>1.01E-17</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="H33" s="18"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="18"/>
       <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="18" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>42</v>
@@ -1793,37 +1820,33 @@
       <c r="C35" s="19">
         <v>1</v>
       </c>
-      <c r="D35" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" s="18"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="26" t="s">
-        <v>60</v>
+      <c r="D35" s="19">
+        <v>20437</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="24">
+        <v>1.01E-17</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="H35" s="18"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="19">
-        <v>1</v>
-      </c>
-      <c r="D36" s="19">
-        <v>955</v>
-      </c>
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="18"/>
       <c r="F36" s="20"/>
-      <c r="G36" s="26"/>
+      <c r="G36" s="18"/>
       <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>42</v>
@@ -1839,33 +1862,43 @@
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="19">
-        <v>1</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="18"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="26" t="s">
+    <row r="39" spans="1:8">
+      <c r="A39" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="19">
+        <v>1</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="18"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="H38" s="18"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="8"/>
-      <c r="D39" s="16"/>
-      <c r="F39" s="17"/>
+      <c r="H39" s="18"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="18"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CP02 PMUI changes to Ingest sheets
Changed ADCP reference designators in ingest CSV's and created ingest
file for D5
</commit_message>
<xml_diff>
--- a/CP02PMUI/Omaha_Cal_Info_CP02PMUI_00001.xlsx
+++ b/CP02PMUI/Omaha_Cal_Info_CP02PMUI_00001.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6800" yWindow="6280" windowWidth="25560" windowHeight="12540" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="6795" yWindow="6285" windowWidth="25560" windowHeight="12540" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>Calibration Cofficient Value</t>
   </si>
   <si>
-    <t>CP02PMUI-RII01-02-ADCPTG000</t>
-  </si>
-  <si>
     <t>CC_depth</t>
   </si>
   <si>
@@ -299,6 +296,9 @@
   <si>
     <t>units = mm</t>
   </si>
+  <si>
+    <t>CP02PMUI-RII01-02-ADCPTG010</t>
+  </si>
 </sst>
 </file>
 
@@ -307,7 +307,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -433,6 +433,7 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -981,25 +982,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" customWidth="1"/>
-    <col min="7" max="8" width="18.5" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="8" width="18.42578125" customWidth="1"/>
     <col min="9" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30">
+    <row r="1" spans="1:13" ht="47.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1008,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1034,12 +1035,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15">
+    <row r="2" spans="1:13">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="10">
         <v>1</v>
@@ -1054,16 +1055,16 @@
         <v>41741</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="I2" s="5">
         <v>93</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K2" s="6"/>
       <c r="L2" s="15"/>
@@ -1092,22 +1093,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.1640625" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1116,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>12</v>
@@ -1129,10 +1130,10 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="18" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="19">
         <v>1</v>
@@ -1141,22 +1142,22 @@
         <v>19336</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="20">
         <v>73000</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="18" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="19">
         <v>1</v>
@@ -1165,7 +1166,7 @@
         <v>19336</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="20">
         <v>40.363405</v>
@@ -1175,10 +1176,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="19">
         <v>1</v>
@@ -1187,7 +1188,7 @@
         <v>19336</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="20">
         <v>-70.775988333333331</v>
@@ -1207,35 +1208,35 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="19">
         <v>1</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="20"/>
       <c r="G6" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H6" s="18"/>
     </row>
-    <row r="7" spans="1:8" ht="15">
+    <row r="7" spans="1:8">
       <c r="A7" s="8"/>
       <c r="D7" s="16"/>
       <c r="F7" s="17"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="19">
         <v>1</v>
@@ -1244,22 +1245,22 @@
         <v>2497</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="22">
         <v>-837.37</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="19">
         <v>1</v>
@@ -1268,7 +1269,7 @@
         <v>2497</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" s="20">
         <v>40.363405</v>
@@ -1278,10 +1279,10 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="19">
         <v>1</v>
@@ -1290,7 +1291,7 @@
         <v>2497</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" s="20">
         <v>-70.775988333333331</v>
@@ -1300,10 +1301,10 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="19">
         <v>1</v>
@@ -1312,22 +1313,22 @@
         <v>2497</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="22">
         <v>2.5849999999999999E-4</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="19">
         <v>1</v>
@@ -1336,22 +1337,22 @@
         <v>2497</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="22">
         <v>-3.3024999999999999E-3</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C13" s="19">
         <v>1</v>
@@ -1360,22 +1361,22 @@
         <v>2497</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="22">
         <v>1.9880000000000001E-4</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="19">
         <v>1</v>
@@ -1384,22 +1385,22 @@
         <v>2497</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14" s="22">
         <v>-3.0292999999999999E-6</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="19">
         <v>1</v>
@@ -1408,13 +1409,13 @@
         <v>2497</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="22">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -1430,10 +1431,10 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="19">
         <v>1</v>
@@ -1442,7 +1443,7 @@
         <v>111</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" s="20">
         <v>40.363405</v>
@@ -1452,10 +1453,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="19">
         <v>1</v>
@@ -1464,7 +1465,7 @@
         <v>111</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F18" s="20">
         <v>-70.775988333333331</v>
@@ -1484,10 +1485,10 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="19">
         <v>1</v>
@@ -1496,7 +1497,7 @@
         <v>100015</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F20" s="20">
         <v>40.363405</v>
@@ -1506,10 +1507,10 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="19">
         <v>1</v>
@@ -1518,7 +1519,7 @@
         <v>100015</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F21" s="20">
         <v>-70.775988333333331</v>
@@ -1538,10 +1539,10 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="19">
         <v>1</v>
@@ -1550,22 +1551,22 @@
         <v>1029</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F23" s="20">
         <v>1.0760000000000001</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H23" s="18"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="19">
         <v>1</v>
@@ -1574,22 +1575,22 @@
         <v>1029</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24" s="20">
         <v>50</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" s="19">
         <v>1</v>
@@ -1598,22 +1599,22 @@
         <v>1029</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F25" s="20">
         <v>53</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="19">
         <v>1</v>
@@ -1622,22 +1623,22 @@
         <v>1029</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F26" s="20">
         <v>50</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H26" s="18"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" s="19">
         <v>1</v>
@@ -1646,22 +1647,22 @@
         <v>1029</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27" s="20">
         <v>3.9E-2</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H27" s="18"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="19">
         <v>1</v>
@@ -1670,22 +1671,22 @@
         <v>1029</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F28" s="20">
         <v>700</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="19">
         <v>1</v>
@@ -1694,22 +1695,22 @@
         <v>1029</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F29" s="20">
         <v>9.0700000000000003E-2</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H29" s="18"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" s="19">
         <v>1</v>
@@ -1718,22 +1719,22 @@
         <v>1029</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F30" s="20">
         <v>1.21E-2</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H30" s="18"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C31" s="19">
         <v>1</v>
@@ -1742,22 +1743,22 @@
         <v>1029</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F31" s="24">
         <v>3.49E-6</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H31" s="18"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" s="19">
         <v>1</v>
@@ -1766,13 +1767,13 @@
         <v>1029</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F32" s="20">
         <v>124</v>
       </c>
       <c r="G32" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H32" s="18"/>
     </row>
@@ -1788,10 +1789,10 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" s="19">
         <v>1</v>
@@ -1800,22 +1801,22 @@
         <v>20437</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F34" s="20">
         <v>1.5</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" s="19">
         <v>1</v>
@@ -1824,13 +1825,13 @@
         <v>20437</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F35" s="24">
         <v>1.01E-17</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H35" s="18"/>
     </row>
@@ -1846,16 +1847,16 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C37" s="19">
         <v>1</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E37" s="18"/>
       <c r="F37" s="20"/>
@@ -1864,21 +1865,21 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="19">
+        <v>1</v>
+      </c>
+      <c r="D39" s="25" t="s">
         <v>62</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="19">
-        <v>1</v>
-      </c>
-      <c r="D39" s="25" t="s">
-        <v>63</v>
       </c>
       <c r="E39" s="18"/>
       <c r="F39" s="20"/>
       <c r="G39" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H39" s="18"/>
     </row>

</xml_diff>